<commit_message>
agregar ejemplos funt mate
</commit_message>
<xml_diff>
--- a/Lecc2/FuncMateCondic.xlsx
+++ b/Lecc2/FuncMateCondic.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ANALISTACP01\Documents\08.CursoExel_Nivel1\Lecc2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReposGit\Excel_InicialDatos\Lecc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B816C2-F5A0-425A-B7EB-0DF63579C85A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F16D8A-A176-4631-A6DF-75A6415B7026}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9ABDD8A0-D50D-4CBA-88BC-C6206BB5B64C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9ABDD8A0-D50D-4CBA-88BC-C6206BB5B64C}"/>
   </bookViews>
   <sheets>
     <sheet name="01_CONDICIONES" sheetId="2" r:id="rId1"/>
     <sheet name="02_ERRORES" sheetId="1" r:id="rId2"/>
+    <sheet name="03,CONTAR.SI" sheetId="3" r:id="rId3"/>
+    <sheet name="04.SUMAR.SI" sheetId="4" r:id="rId4"/>
+    <sheet name="05.SI.CONJUNTO" sheetId="5" r:id="rId5"/>
+    <sheet name="06.DESAFIO1" sheetId="6" r:id="rId6"/>
+    <sheet name="07.DESAFIO2" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'02_ERRORES'!$A$25:$B$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'02_ERRORES'!$B$33:$D$44</definedName>
+    <definedName name="data">'03,CONTAR.SI'!$A$10:$B$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,30 +42,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>COMPARACION</t>
   </si>
@@ -88,39 +72,6 @@
     <t>COD</t>
   </si>
   <si>
-    <t>VALOR</t>
-  </si>
-  <si>
-    <t>ABC1</t>
-  </si>
-  <si>
-    <t>BCD2</t>
-  </si>
-  <si>
-    <t>CDE3</t>
-  </si>
-  <si>
-    <t>ABC2</t>
-  </si>
-  <si>
-    <t>BCD3</t>
-  </si>
-  <si>
-    <t>CDE4</t>
-  </si>
-  <si>
-    <t>ABC3</t>
-  </si>
-  <si>
-    <t>BCD4</t>
-  </si>
-  <si>
-    <t>CUANTO SUMAS LOS 3 CON EL VALOR MÁS ALTO</t>
-  </si>
-  <si>
-    <t>CUANTO SUMAN LOS 3 CON EL VALOR MÁS BAJO</t>
-  </si>
-  <si>
     <t>OPERADORES DE COMPARACION</t>
   </si>
   <si>
@@ -230,16 +181,131 @@
   </si>
   <si>
     <t>ES DISTINTO</t>
+  </si>
+  <si>
+    <t>CUANDO USAR SUBTOTALES/ SUMA / AGREGAR</t>
+  </si>
+  <si>
+    <t>=SUBTOTALES('OPERACION','RANGO')</t>
+  </si>
+  <si>
+    <t>=SUMA('RANGO SUMA')</t>
+  </si>
+  <si>
+    <t>=AGREGAR('OPERACION','QUE IGNORAR', 'RANGO OPERACION')</t>
+  </si>
+  <si>
+    <t>VALOR FILTRA</t>
+  </si>
+  <si>
+    <t>VALOR TOTAL</t>
+  </si>
+  <si>
+    <t>1. EN LA SIGUIENTE TABLA SOLO DESEO SUMAR LAS FILAS VISIBLES DIF ENTRE SUMA Y SUBTOTALES</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>NOTA\</t>
+  </si>
+  <si>
+    <t>SUMA/PROMEDIA/CUENTA SOLO LAS FILAS VISIBLES</t>
+  </si>
+  <si>
+    <t>SUMA TODO ESTE VISIBLE O NO</t>
+  </si>
+  <si>
+    <t>DA LA POSIBILIDAD DE ELEGIR LA OPERACION Y QUE SE QUIERE IGNORAR</t>
+  </si>
+  <si>
+    <t>SUBTOTALES</t>
+  </si>
+  <si>
+    <t>SUMA</t>
+  </si>
+  <si>
+    <t>PROMEDIO</t>
+  </si>
+  <si>
+    <t>NOTA: SIEMPRE SE DEBE CONSIDERAR QUE TIPO DE ANALISIS SE DESEA DESARROLLAR PREVIO APLICAR ESTAS FORMULAS</t>
+  </si>
+  <si>
+    <t>CONTAR FILAS CON VALORES</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total de celdas en rango</t>
+  </si>
+  <si>
+    <t>Celdas blancas</t>
+  </si>
+  <si>
+    <t>Celdas que no son blancas</t>
+  </si>
+  <si>
+    <t>Valores Numericos</t>
+  </si>
+  <si>
+    <t>=3+4*4^3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>primero se suma</t>
+  </si>
+  <si>
+    <t>luego se multiplicaa</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
+  </si>
+  <si>
+    <t>TOTAL SOLO DE LOS VALORES PARCIALES\</t>
+  </si>
+  <si>
+    <t>AGREGAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,13 +343,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="63"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -330,10 +421,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -353,8 +445,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -500,8 +607,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="208906" y="192471"/>
-          <a:ext cx="3296293" cy="603994"/>
+          <a:off x="208906" y="184851"/>
+          <a:ext cx="3397258" cy="581134"/>
           <a:chOff x="2791304" y="276225"/>
           <a:chExt cx="4697162" cy="866820"/>
         </a:xfrm>
@@ -955,16 +1062,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>97155</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -979,8 +1086,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9105900" y="3371850"/>
-          <a:ext cx="1438275" cy="1028700"/>
+          <a:off x="11384280" y="1447800"/>
+          <a:ext cx="1485900" cy="981075"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1146,8 +1253,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="208906" y="192471"/>
-          <a:ext cx="3296293" cy="603994"/>
+          <a:off x="208906" y="184851"/>
+          <a:ext cx="3359158" cy="581134"/>
           <a:chOff x="2791304" y="276225"/>
           <a:chExt cx="4697162" cy="866820"/>
         </a:xfrm>
@@ -1335,14 +1442,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1453515</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>325755</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
@@ -1373,58 +1480,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6105525" y="0"/>
-          <a:ext cx="1752600" cy="525780"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>475689</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagen 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F7BE8C-4615-4D84-B645-BF79036B2185}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6391275" y="552450"/>
-          <a:ext cx="1380564" cy="600075"/>
+          <a:off x="6261735" y="0"/>
+          <a:ext cx="1813560" cy="510540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1436,15 +1493,65 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:colOff>306705</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>308049</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F7BE8C-4615-4D84-B645-BF79036B2185}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6616065" y="537210"/>
+          <a:ext cx="1441524" cy="569595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1127760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1476,8 +1583,61 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4933950" y="171450"/>
-          <a:ext cx="914400" cy="914400"/>
+          <a:off x="4991100" y="156210"/>
+          <a:ext cx="944880" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1142505</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>329070</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Gráfico 10" descr="Inteligencia artificial">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4715D013-3AC4-4E01-9DC8-BC5F8455E3A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3062745" y="0"/>
+          <a:ext cx="946785" cy="883920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1489,22 +1649,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>731025</xdr:colOff>
+      <xdr:colOff>265710</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>78105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>550050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>96165</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>40005</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Gráfico 10" descr="Inteligencia artificial">
+        <xdr:cNvPr id="12" name="Gráfico 11" descr="Pared de ladrillo de edificio">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4715D013-3AC4-4E01-9DC8-BC5F8455E3A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7401E94-C12E-497F-9E3D-759E8EA68050}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1513,13 +1673,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1529,61 +1689,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2607450" y="0"/>
-          <a:ext cx="914400" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>776250</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>233325</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Gráfico 11" descr="Pared de ladrillo de edificio">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7401E94-C12E-497F-9E3D-759E8EA68050}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3414675" y="123825"/>
-          <a:ext cx="914400" cy="914400"/>
+          <a:off x="3946170" y="78105"/>
+          <a:ext cx="958215" cy="876300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1806,16 +1913,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1830,13 +1937,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="1276350"/>
-          <a:ext cx="2324100" cy="1562100"/>
+          <a:off x="11357610" y="803910"/>
+          <a:ext cx="2415540" cy="1510665"/>
         </a:xfrm>
         <a:prstGeom prst="cloudCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -85686"/>
-            <a:gd name="adj2" fmla="val 82771"/>
+            <a:gd name="adj1" fmla="val -102405"/>
+            <a:gd name="adj2" fmla="val 41913"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -1873,6 +1980,657 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>583425</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177660</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Gráfico 18" descr="Cerrar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{003AC88B-43CA-4EF5-A597-2E6AB43017E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId12"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3909060" y="8884920"/>
+          <a:ext cx="354825" cy="337680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>120015</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Gráfico 20" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F7E5430-2F73-4387-8328-3619A0F7B3BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId10"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3718560" y="9258300"/>
+          <a:ext cx="381000" cy="363855"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215265</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>36450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA1A332C-0848-4489-91C1-1DAC588CFABA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8140065" cy="1133730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00203C"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00203C"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>208906</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>398144</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>42760</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="Grupo 2" descr="&quot;&quot;" title="Lista de comprobación de elementos de vacaciones">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5B307ED-ECB9-4FBA-B083-7A416E05992F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="208906" y="184851"/>
+          <a:ext cx="3359158" cy="589429"/>
+          <a:chOff x="2791304" y="276225"/>
+          <a:chExt cx="4697162" cy="879193"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="4" name="Lista de comprobación de elementos de vacaciones" descr="&quot;&quot;" title="Lista de comprobación de elementos de vacaciones">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6639CAE3-C424-4233-8812-18772EAD1BC9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2799789" y="276225"/>
+            <a:ext cx="4688677" cy="879193"/>
+            <a:chOff x="3686175" y="152400"/>
+            <a:chExt cx="2978527" cy="879193"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Cuadro de texto 321">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{255D4F24-69DB-44E1-BFFD-086E8D89E666}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3686175" y="152400"/>
+              <a:ext cx="2667000" cy="571500"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:r>
+                <a:rPr lang="es" sz="2000" b="1" spc="50" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mj-lt"/>
+                </a:rPr>
+                <a:t>LECCION 2</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:endParaRPr lang="en-US" sz="2000" b="1" spc="50" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Cuadro de texto 322">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4161445F-E49E-4773-A17E-5F274C114545}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3695191" y="704689"/>
+              <a:ext cx="2969511" cy="326904"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" spc="200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>CONTAR.SI</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="Conector recto 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DF37FCD-D5C3-460F-B2BA-2D0C4ADE697D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2791304" y="768343"/>
+            <a:ext cx="4383015" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>668655</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A303DCE-E842-405F-8DFB-4BC0FEAE5F68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6216015" y="0"/>
+          <a:ext cx="1813560" cy="510540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>100965</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>750009</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>24765</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B03DD51D-2669-4C5F-88D2-52F5D6B40E8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6440805" y="552450"/>
+          <a:ext cx="1441524" cy="569595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Gráfico 9" descr="Publicidad">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17BCE7DB-D201-42D9-9BB9-714F18936A6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4480560" y="0"/>
+          <a:ext cx="944880" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>357645</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>511950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Gráfico 10" descr="Inteligencia artificial">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E910731F-A393-449D-8592-40BECB50E2F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3527565" y="0"/>
+          <a:ext cx="946785" cy="883920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>578130</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>743865</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Gráfico 11" descr="Pared de ladrillo de edificio">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7FBB7A6-7CC6-4D55-9695-A2BA36D56235}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5333010" y="0"/>
+          <a:ext cx="958215" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2221,170 +2979,212 @@
   </sheetPr>
   <dimension ref="B9:K31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="D11" s="13" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="D12" s="10" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="K12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="D13" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="K13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="D14" s="10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="K14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="D15" s="10" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="K15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:11" ht="18" x14ac:dyDescent="0.35">
       <c r="D16" s="10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
-    </row>
-    <row r="24" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>45</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <f>(G19+H19)*F19</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B24" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>2</v>
       </c>
@@ -2392,7 +3192,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E26" t="b">
         <f>B26=C26</f>
@@ -2403,7 +3203,7 @@
         <v>=B26=C26</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>5</v>
       </c>
@@ -2411,7 +3211,7 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E27" t="b">
         <f>B27&gt;C27</f>
@@ -2422,7 +3222,7 @@
         <v>=B27&gt;C27</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>3</v>
       </c>
@@ -2430,7 +3230,7 @@
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E28" t="b">
         <f>B28&lt;C28</f>
@@ -2441,7 +3241,7 @@
         <v>=B28&lt;C28</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>5</v>
       </c>
@@ -2449,7 +3249,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E29" t="b">
         <f>B29&gt;=C29</f>
@@ -2460,7 +3260,7 @@
         <v>=B29&gt;=C29</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>4</v>
       </c>
@@ -2468,7 +3268,7 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E30" t="b">
         <f>B30&lt;=C30</f>
@@ -2479,7 +3279,7 @@
         <v>=B30&lt;=C30</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>8</v>
       </c>
@@ -2487,7 +3287,7 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E31" t="b">
         <f>B31&lt;&gt;C31</f>
@@ -2511,27 +3311,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8A0F3B-36C2-4A71-9B9D-1234CCC94A5B}">
-  <dimension ref="A9:F33"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A9:G56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
@@ -2545,8 +3346,11 @@
         <v>4</v>
       </c>
       <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>2324</v>
       </c>
@@ -2559,8 +3363,11 @@
       <c r="E12" s="7">
         <v>2324</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="7">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>3543</v>
       </c>
@@ -2573,8 +3380,11 @@
       <c r="E13" s="7">
         <v>3543</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="7">
+        <v>3543</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>34546</v>
       </c>
@@ -2587,8 +3397,11 @@
       <c r="E14" s="7">
         <v>34546</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="7">
+        <v>34546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="e">
         <v>#N/A</v>
       </c>
@@ -2601,8 +3414,15 @@
       <c r="E15" s="7" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15">
+        <f>+SUBTOTAL(9,G12:G14)</f>
+        <v>40413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="e">
         <v>#VALUE!</v>
       </c>
@@ -2615,8 +3435,16 @@
       <c r="E16" s="7" t="e">
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="7">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="7">
+        <v>3543</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -2636,9 +3464,20 @@
         <f>_xlfn.AGGREGATE(9,6,E12:E16)</f>
         <v>40413</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="7">
+        <v>34546</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="1">
+        <f>+SUBTOTAL(1,G16:G18)</f>
+        <v>13471</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -2659,95 +3498,496 @@
         <v>=AGREGAR(9;6;E12:E16)</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="15">
+        <f>_xlfn.AGGREGATE(9,6,E12:E16)</f>
+        <v>40413</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21">
+        <f>_xlfn.AGGREGATE(9,0,G12:G19)</f>
+        <v>80826</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f>SUM(G16:G18)+SUM(G12:G14)</f>
+        <v>80826</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A24" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A31" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>2342</v>
-      </c>
-      <c r="D26">
-        <f t="array" ref="D26">SUM(LARGE(B26:B33,{1,2,3}))</f>
-        <v>705020</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27">
-        <v>234235</v>
-      </c>
-      <c r="D27" cm="1">
-        <f t="array" ref="D27">SUM(SMALL(B26:B33,{1,2,3}))</f>
-        <v>2926</v>
-      </c>
-      <c r="E27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29">
-        <v>2352</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C33" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="17">
+        <v>4313</v>
+      </c>
+      <c r="D34" s="17">
+        <v>4313</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="17">
+        <v>22</v>
+      </c>
+      <c r="D35" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="17">
+        <v>22</v>
+      </c>
+      <c r="D36" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="17">
+        <v>3231</v>
+      </c>
+      <c r="D37" s="17">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="17">
+        <v>3213</v>
+      </c>
+      <c r="D38" s="17">
+        <v>3213</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="17">
+        <v>232</v>
+      </c>
+      <c r="D39" s="17">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="17">
+        <v>3323</v>
+      </c>
+      <c r="D40" s="17">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="17">
+        <v>125</v>
+      </c>
+      <c r="D41" s="17">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="17">
+        <v>3323</v>
+      </c>
+      <c r="D42" s="17">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="17">
+        <v>232</v>
+      </c>
+      <c r="D43" s="17">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="17">
+        <v>2332</v>
+      </c>
+      <c r="D44" s="17">
+        <v>2332</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B46" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="18">
+        <f>SUBTOTAL(9,C34:C44)</f>
+        <v>7125</v>
+      </c>
+      <c r="D46" s="19">
+        <f>SUBTOTAL(1,D34:D44)</f>
+        <v>1425</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C46)</f>
+        <v>=SUBTOTALES(9;C34:C44)</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B47" s="10"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="20"/>
+    </row>
+    <row r="48" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B48" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="18">
+        <f>SUM(C34:C44)</f>
+        <v>20368</v>
+      </c>
+      <c r="D48" s="19">
+        <f>AVERAGE(D34:D44)</f>
+        <v>1851.6363636363637</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C48)</f>
+        <v>=SUMA(C34:C44)</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C49" t="b">
+        <f>C48=C46</f>
+        <v>0</v>
+      </c>
+      <c r="D49" t="b">
+        <f>D48=D46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B50" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="18">
+        <f>_xlfn.AGGREGATE(9,3,C34:C44)</f>
+        <v>7125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B51" s="4"/>
+      <c r="C51" s="18"/>
+    </row>
+    <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B52" s="4"/>
+      <c r="C52" s="18"/>
+    </row>
+    <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B53" s="4"/>
+      <c r="C53" s="18">
+        <f>SUM(C38:C43)</f>
+        <v>10448</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="B54" s="4"/>
+      <c r="C54" s="18">
+        <f>SUBTOTAL(9,C38:C43)</f>
+        <v>7125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A56" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B33:D44" xr:uid="{38F4915D-6D55-4ED2-9332-A64584F67B15}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="B"/>
+        <filter val="CC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C27F91F-BB01-4654-A81F-C948EDDBAA11}">
+  <dimension ref="A8:E24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="8" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A8" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <f>ROWS(data)*COLUMNS(data)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
+        <v>525</v>
+      </c>
+      <c r="B11" s="23">
+        <v>718</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11">
+        <f>COUNTBLANK(data)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="D12" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12">
+        <f>COUNTA(data)</f>
         <v>14</v>
       </c>
-      <c r="B30">
-        <v>235532</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31">
-        <v>235253</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32">
-        <v>23523</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33">
-        <v>532</v>
-      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="23">
+        <v>3</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="D13" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13">
+        <f>COUNT(data)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="23">
+        <v>552</v>
+      </c>
+      <c r="B14" s="23">
+        <v>911</v>
+      </c>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
+        <v>250</v>
+      </c>
+      <c r="B15" s="23">
+        <v>98</v>
+      </c>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23" t="e">
+        <f>B15/B17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="23" t="e">
+        <f>mydata</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FA955F-7098-48A1-AB51-7544B84DEB56}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1129748-9DF1-4EB8-8938-58EFF12AEA84}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66D965B-CD9F-4069-906C-76269E752F0A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97223706-25BC-4B5C-AFEB-83702A354A86}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>